<commit_message>
finish sirt for c++ version
</commit_message>
<xml_diff>
--- a/final/research/Book1.xlsx
+++ b/final/research/Book1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26812"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhvan5481/Box Sync/EE382C-multiple-cores-computing/final/research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dinhvan5481/Documents/projects/ee360p-multiple-cores-computing/final/research/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>URL</t>
   </si>
@@ -78,6 +81,15 @@
   </si>
   <si>
     <t>Matlab code for MRI</t>
+  </si>
+  <si>
+    <t>http://www2.compute.dtu.dk/~pcha/AIRtools/AIRtoolsManual.pdf</t>
+  </si>
+  <si>
+    <t>Tool box for matlab</t>
+  </si>
+  <si>
+    <t>https://tomroelandts.com/articles/do-not-ignore-the-astra-toolbox</t>
   </si>
 </sst>
 </file>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -507,6 +519,19 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>